<commit_message>
Bad data checks and warning message, show both original and final data
</commit_message>
<xml_diff>
--- a/LCx Example Data.xlsx
+++ b/LCx Example Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carrGJ/Documents/ShinyByGIT/LogisticAbbott/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114843C1-4EB8-8246-8208-1DC79CAF2BF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402CEC4B-B18F-8C4A-97B3-393F75394793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ECx data + Bkgd.txt" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,21 @@
     <sheet name="ECx steep + Bkgd.txt" sheetId="3" r:id="rId3"/>
     <sheet name="ECx steep.txt" sheetId="4" r:id="rId4"/>
     <sheet name="ECx steep2 + Bkgd.txt" sheetId="5" r:id="rId5"/>
-    <sheet name="ECx doses too low" sheetId="10" r:id="rId6"/>
-    <sheet name="ECx steep2.txt" sheetId="6" r:id="rId7"/>
-    <sheet name="hamilton 1B.txt" sheetId="7" r:id="rId8"/>
-    <sheet name="hamilton 1C.txt" sheetId="8" r:id="rId9"/>
-    <sheet name="SKdata.txt" sheetId="9" r:id="rId10"/>
+    <sheet name="ECx Flat" sheetId="11" r:id="rId6"/>
+    <sheet name="ECx doses too low" sheetId="10" r:id="rId7"/>
+    <sheet name="ECx steep2.txt" sheetId="6" r:id="rId8"/>
+    <sheet name="hamilton 1B.txt" sheetId="7" r:id="rId9"/>
+    <sheet name="ECx Invalid data" sheetId="13" r:id="rId10"/>
+    <sheet name="hamilton 1C.txt" sheetId="8" r:id="rId11"/>
+    <sheet name="ECx names" sheetId="12" r:id="rId12"/>
+    <sheet name="SKdata.txt" sheetId="9" r:id="rId13"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="6">
   <si>
     <t>doses</t>
   </si>
@@ -38,6 +41,15 @@
   </si>
   <si>
     <t>sizes</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -515,10 +527,277 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714B54DB-317D-B74D-A0C3-8964F4A463E6}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>15.54</v>
+      </c>
+      <c r="B3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>20.47</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>27.92</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>55.52</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>15.54</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>20.47</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>27.92</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>35.979999999999997</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>55.52</v>
+      </c>
+      <c r="B7" s="2">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82E30CD-0F7F-874F-BAE5-426150A3E5B9}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -932,11 +1211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601EA01A-E059-1147-BFB5-807AACA5A4D8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CE48C3-AEC5-364B-B88D-34103359790C}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -960,7 +1239,7 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -971,7 +1250,7 @@
         <v>20</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -982,7 +1261,7 @@
         <v>20</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -993,7 +1272,7 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1004,7 +1283,7 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1013,6 +1292,87 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601EA01A-E059-1147-BFB5-807AACA5A4D8}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1091,7 +1451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1179,94 +1539,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>15.54</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>20.47</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>27.92</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>35.979999999999997</v>
-      </c>
-      <c r="B6" s="2">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>55.52</v>
-      </c>
-      <c r="B7" s="2">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>